<commit_message>
Exim save to clean, not semi-clean.
</commit_message>
<xml_diff>
--- a/Output/Assistance/USAspending_selected_assistance_critical_tech.xlsx
+++ b/Output/Assistance/USAspending_selected_assistance_critical_tech.xlsx
@@ -11720,6 +11720,11 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
@@ -11729,11 +11734,6 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -11768,49 +11768,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-    </border>
-    <border>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -11860,6 +11817,49 @@
       </right>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+    </border>
+    <border>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
       <left style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </left>
@@ -11890,60 +11890,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12294,22 +12294,22 @@
       <c r="A2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -12317,22 +12317,22 @@
       <c r="A3" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -12340,22 +12340,22 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="b">
+      <c r="B4" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="b">
+      <c r="C4" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -12363,22 +12363,22 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -12386,22 +12386,22 @@
       <c r="A6" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="4" t="s">
         <v>1972</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="4" t="s">
         <v>1972</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="12" t="s">
         <v>0</v>
       </c>
     </row>
@@ -12409,18 +12409,18 @@
       <c r="A7" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="8"/>
+      <c r="F7" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -12446,299 +12446,299 @@
     <row r="15" ht="15.75" customHeight="1"/>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="H17" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H20" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="I20" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10" t="s">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="9" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" ht="224.25" customHeight="1">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F26" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G26" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H26" s="9" t="s">
+      <c r="H26" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I26" s="9" t="s">
+      <c r="I26" s="14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F27" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I27" s="9" t="s">
+      <c r="I27" s="14" t="s">
         <v>7</v>
       </c>
     </row>
@@ -12929,37 +12929,37 @@
       <c r="A1" s="15" t="s">
         <v>1973</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="12" t="s">
         <v>1974</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="12" t="s">
         <v>1975</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="12" t="s">
         <v>1976</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="12" t="s">
         <v>1977</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="12" t="s">
         <v>1978</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="12" t="s">
         <v>1979</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="12" t="s">
         <v>1980</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="12" t="s">
         <v>1981</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="12" t="s">
         <v>1982</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="12" t="s">
         <v>1983</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="12" t="s">
         <v>1984</v>
       </c>
       <c r="M1" s="21" t="s">
@@ -12968,358 +12968,358 @@
       <c r="N1" s="22" t="s">
         <v>1986</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="12" t="s">
         <v>1987</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="12" t="s">
         <v>1988</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="12" t="s">
         <v>1989</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="12" t="s">
         <v>1990</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="12" t="s">
         <v>1991</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="12" t="s">
         <v>1992</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="12" t="s">
         <v>1993</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="12" t="s">
         <v>1994</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="12" t="s">
         <v>1995</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="12" t="s">
         <v>1996</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="12" t="s">
         <v>1997</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" s="12" t="s">
         <v>1998</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="12" t="s">
         <v>1999</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AB1" s="12" t="s">
         <v>2000</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" s="12" t="s">
         <v>2001</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AD1" s="12" t="s">
         <v>2002</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AE1" s="12" t="s">
         <v>2003</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AF1" s="12" t="s">
         <v>2004</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AG1" s="12" t="s">
         <v>2005</v>
       </c>
-      <c r="AH1" s="7" t="s">
+      <c r="AH1" s="12" t="s">
         <v>2006</v>
       </c>
-      <c r="AI1" s="7" t="s">
+      <c r="AI1" s="12" t="s">
         <v>2007</v>
       </c>
-      <c r="AJ1" s="7" t="s">
+      <c r="AJ1" s="12" t="s">
         <v>2008</v>
       </c>
-      <c r="AK1" s="7" t="s">
+      <c r="AK1" s="12" t="s">
         <v>2009</v>
       </c>
-      <c r="AL1" s="7" t="s">
+      <c r="AL1" s="12" t="s">
         <v>2010</v>
       </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AM1" s="12" t="s">
         <v>2011</v>
       </c>
-      <c r="AN1" s="7" t="s">
+      <c r="AN1" s="12" t="s">
         <v>2012</v>
       </c>
-      <c r="AO1" s="7" t="s">
+      <c r="AO1" s="12" t="s">
         <v>2013</v>
       </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AP1" s="12" t="s">
         <v>2014</v>
       </c>
-      <c r="AQ1" s="7" t="s">
+      <c r="AQ1" s="12" t="s">
         <v>2015</v>
       </c>
-      <c r="AR1" s="7" t="s">
+      <c r="AR1" s="12" t="s">
         <v>2016</v>
       </c>
-      <c r="AS1" s="7" t="s">
+      <c r="AS1" s="12" t="s">
         <v>2017</v>
       </c>
-      <c r="AT1" s="7" t="s">
+      <c r="AT1" s="12" t="s">
         <v>2018</v>
       </c>
-      <c r="AU1" s="7" t="s">
+      <c r="AU1" s="12" t="s">
         <v>2019</v>
       </c>
-      <c r="AV1" s="7" t="s">
+      <c r="AV1" s="12" t="s">
         <v>2020</v>
       </c>
-      <c r="AW1" s="7" t="s">
+      <c r="AW1" s="12" t="s">
         <v>2021</v>
       </c>
-      <c r="AX1" s="7" t="s">
+      <c r="AX1" s="12" t="s">
         <v>2022</v>
       </c>
-      <c r="AY1" s="7" t="s">
+      <c r="AY1" s="12" t="s">
         <v>2023</v>
       </c>
-      <c r="AZ1" s="7" t="s">
+      <c r="AZ1" s="12" t="s">
         <v>2024</v>
       </c>
-      <c r="BA1" s="7" t="s">
+      <c r="BA1" s="12" t="s">
         <v>2025</v>
       </c>
-      <c r="BB1" s="7" t="s">
+      <c r="BB1" s="12" t="s">
         <v>2026</v>
       </c>
-      <c r="BC1" s="7" t="s">
+      <c r="BC1" s="12" t="s">
         <v>2027</v>
       </c>
-      <c r="BD1" s="7" t="s">
+      <c r="BD1" s="12" t="s">
         <v>2028</v>
       </c>
-      <c r="BE1" s="7" t="s">
+      <c r="BE1" s="12" t="s">
         <v>2029</v>
       </c>
-      <c r="BF1" s="7" t="s">
+      <c r="BF1" s="12" t="s">
         <v>2030</v>
       </c>
-      <c r="BG1" s="7" t="s">
+      <c r="BG1" s="12" t="s">
         <v>2031</v>
       </c>
-      <c r="BH1" s="7" t="s">
+      <c r="BH1" s="12" t="s">
         <v>2032</v>
       </c>
-      <c r="BI1" s="7" t="s">
+      <c r="BI1" s="12" t="s">
         <v>2033</v>
       </c>
-      <c r="BJ1" s="7" t="s">
+      <c r="BJ1" s="12" t="s">
         <v>2034</v>
       </c>
-      <c r="BK1" s="7" t="s">
+      <c r="BK1" s="12" t="s">
         <v>2035</v>
       </c>
-      <c r="BL1" s="7" t="s">
+      <c r="BL1" s="12" t="s">
         <v>2036</v>
       </c>
-      <c r="BM1" s="7" t="s">
+      <c r="BM1" s="12" t="s">
         <v>2037</v>
       </c>
-      <c r="BN1" s="7" t="s">
+      <c r="BN1" s="12" t="s">
         <v>2038</v>
       </c>
-      <c r="BO1" s="7" t="s">
+      <c r="BO1" s="12" t="s">
         <v>2039</v>
       </c>
-      <c r="BP1" s="7" t="s">
+      <c r="BP1" s="12" t="s">
         <v>2040</v>
       </c>
-      <c r="BQ1" s="7" t="s">
+      <c r="BQ1" s="12" t="s">
         <v>2041</v>
       </c>
-      <c r="BR1" s="7" t="s">
+      <c r="BR1" s="12" t="s">
         <v>2042</v>
       </c>
-      <c r="BS1" s="7" t="s">
+      <c r="BS1" s="12" t="s">
         <v>2043</v>
       </c>
-      <c r="BT1" s="7" t="s">
+      <c r="BT1" s="12" t="s">
         <v>2044</v>
       </c>
-      <c r="BU1" s="7" t="s">
+      <c r="BU1" s="12" t="s">
         <v>2045</v>
       </c>
-      <c r="BV1" s="7" t="s">
+      <c r="BV1" s="12" t="s">
         <v>2046</v>
       </c>
-      <c r="BW1" s="7" t="s">
+      <c r="BW1" s="12" t="s">
         <v>2047</v>
       </c>
-      <c r="BX1" s="7" t="s">
+      <c r="BX1" s="12" t="s">
         <v>2048</v>
       </c>
-      <c r="BY1" s="7" t="s">
+      <c r="BY1" s="12" t="s">
         <v>2049</v>
       </c>
-      <c r="BZ1" s="7" t="s">
+      <c r="BZ1" s="12" t="s">
         <v>2050</v>
       </c>
-      <c r="CA1" s="7" t="s">
+      <c r="CA1" s="12" t="s">
         <v>2051</v>
       </c>
-      <c r="CB1" s="7" t="s">
+      <c r="CB1" s="12" t="s">
         <v>2052</v>
       </c>
-      <c r="CC1" s="7" t="s">
+      <c r="CC1" s="12" t="s">
         <v>2053</v>
       </c>
-      <c r="CD1" s="7" t="s">
+      <c r="CD1" s="12" t="s">
         <v>2054</v>
       </c>
-      <c r="CE1" s="7" t="s">
+      <c r="CE1" s="12" t="s">
         <v>2055</v>
       </c>
-      <c r="CF1" s="7" t="s">
+      <c r="CF1" s="12" t="s">
         <v>2056</v>
       </c>
-      <c r="CG1" s="7" t="s">
+      <c r="CG1" s="12" t="s">
         <v>2057</v>
       </c>
-      <c r="CH1" s="7" t="s">
+      <c r="CH1" s="12" t="s">
         <v>2058</v>
       </c>
-      <c r="CI1" s="7" t="s">
+      <c r="CI1" s="12" t="s">
         <v>2059</v>
       </c>
-      <c r="CJ1" s="7" t="s">
+      <c r="CJ1" s="12" t="s">
         <v>2060</v>
       </c>
-      <c r="CK1" s="7" t="s">
+      <c r="CK1" s="12" t="s">
         <v>2061</v>
       </c>
-      <c r="CL1" s="7" t="s">
+      <c r="CL1" s="12" t="s">
         <v>2062</v>
       </c>
-      <c r="CM1" s="7" t="s">
+      <c r="CM1" s="12" t="s">
         <v>2063</v>
       </c>
-      <c r="CN1" s="7" t="s">
+      <c r="CN1" s="12" t="s">
         <v>2064</v>
       </c>
-      <c r="CO1" s="7" t="s">
+      <c r="CO1" s="12" t="s">
         <v>2065</v>
       </c>
-      <c r="CP1" s="7" t="s">
+      <c r="CP1" s="12" t="s">
         <v>2066</v>
       </c>
-      <c r="CQ1" s="7" t="s">
+      <c r="CQ1" s="12" t="s">
         <v>2067</v>
       </c>
-      <c r="CR1" s="7" t="s">
+      <c r="CR1" s="12" t="s">
         <v>2068</v>
       </c>
-      <c r="CS1" s="7" t="s">
+      <c r="CS1" s="12" t="s">
         <v>2069</v>
       </c>
-      <c r="CT1" s="7" t="s">
+      <c r="CT1" s="12" t="s">
         <v>2070</v>
       </c>
-      <c r="CU1" s="7" t="s">
+      <c r="CU1" s="12" t="s">
         <v>2071</v>
       </c>
-      <c r="CV1" s="7" t="s">
+      <c r="CV1" s="12" t="s">
         <v>2072</v>
       </c>
-      <c r="CW1" s="7" t="s">
+      <c r="CW1" s="12" t="s">
         <v>2073</v>
       </c>
-      <c r="CX1" s="7" t="s">
+      <c r="CX1" s="12" t="s">
         <v>2074</v>
       </c>
-      <c r="CY1" s="7" t="s">
+      <c r="CY1" s="12" t="s">
         <v>2075</v>
       </c>
-      <c r="CZ1" s="7" t="s">
+      <c r="CZ1" s="12" t="s">
         <v>2076</v>
       </c>
-      <c r="DA1" s="7" t="s">
+      <c r="DA1" s="12" t="s">
         <v>2077</v>
       </c>
-      <c r="DB1" s="7" t="s">
+      <c r="DB1" s="12" t="s">
         <v>2078</v>
       </c>
-      <c r="DC1" s="7" t="s">
+      <c r="DC1" s="12" t="s">
         <v>2079</v>
       </c>
-      <c r="DD1" s="7" t="s">
+      <c r="DD1" s="12" t="s">
         <v>2080</v>
       </c>
-      <c r="DE1" s="7" t="s">
+      <c r="DE1" s="12" t="s">
         <v>2081</v>
       </c>
       <c r="DF1" s="15" t="s">
         <v>2082</v>
       </c>
-      <c r="DG1" s="7" t="s">
+      <c r="DG1" s="12" t="s">
         <v>2083</v>
       </c>
-      <c r="DH1" s="7" t="s">
+      <c r="DH1" s="12" t="s">
         <v>2084</v>
       </c>
-      <c r="DI1" s="7" t="s">
+      <c r="DI1" s="12" t="s">
         <v>2085</v>
       </c>
-      <c r="DJ1" s="7" t="s">
+      <c r="DJ1" s="12" t="s">
         <v>2086</v>
       </c>
-      <c r="DK1" s="7" t="s">
+      <c r="DK1" s="12" t="s">
         <v>2087</v>
       </c>
-      <c r="DL1" s="7" t="s">
+      <c r="DL1" s="12" t="s">
         <v>2088</v>
       </c>
-      <c r="DM1" s="7" t="s">
+      <c r="DM1" s="12" t="s">
         <v>2089</v>
       </c>
-      <c r="DN1" s="7" t="s">
+      <c r="DN1" s="12" t="s">
         <v>2090</v>
       </c>
-      <c r="DO1" s="7" t="s">
+      <c r="DO1" s="12" t="s">
         <v>2091</v>
       </c>
-      <c r="DP1" s="7" t="s">
+      <c r="DP1" s="12" t="s">
         <v>2092</v>
       </c>
-      <c r="DQ1" s="7" t="s">
+      <c r="DQ1" s="12" t="s">
         <v>2093</v>
       </c>
-      <c r="DR1" s="7" t="s">
+      <c r="DR1" s="12" t="s">
         <v>2094</v>
       </c>
-      <c r="DS1" s="7" t="s">
+      <c r="DS1" s="12" t="s">
         <v>2095</v>
       </c>
-      <c r="DT1" s="7" t="s">
+      <c r="DT1" s="12" t="s">
         <v>2096</v>
       </c>
-      <c r="DU1" s="7" t="s">
+      <c r="DU1" s="12" t="s">
         <v>2097</v>
       </c>
-      <c r="DV1" s="7" t="s">
+      <c r="DV1" s="12" t="s">
         <v>2098</v>
       </c>
-      <c r="DW1" s="7" t="s">
+      <c r="DW1" s="12" t="s">
         <v>2099</v>
       </c>
-      <c r="DX1" s="7" t="s">
+      <c r="DX1" s="12" t="s">
         <v>2100</v>
       </c>
-      <c r="DY1" s="7" t="s">
+      <c r="DY1" s="12" t="s">
         <v>2101</v>
       </c>
-      <c r="DZ1" s="7" t="s">
+      <c r="DZ1" s="12" t="s">
         <v>2102</v>
       </c>
-      <c r="EA1" s="7" t="s">
+      <c r="EA1" s="12" t="s">
         <v>2103</v>
       </c>
-      <c r="EB1" s="7" t="s">
+      <c r="EB1" s="12" t="s">
         <v>2104</v>
       </c>
       <c r="EC1" t="s">

</xml_diff>

<commit_message>
Moving agency_assistance to label.
</commit_message>
<xml_diff>
--- a/Output/Assistance/USAspending_selected_assistance_critical_tech.xlsx
+++ b/Output/Assistance/USAspending_selected_assistance_critical_tech.xlsx
@@ -11721,6 +11721,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
@@ -11728,12 +11734,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <b/>
     </font>
   </fonts>
   <fills count="4">
@@ -11768,6 +11768,38 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+    </border>
+    <border>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -11828,38 +11860,6 @@
       </bottom>
     </border>
     <border>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-    </border>
-    <border>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
       <left style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </left>
@@ -11887,63 +11887,63 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12294,22 +12294,22 @@
       <c r="A2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -12317,22 +12317,22 @@
       <c r="A3" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="14" t="s">
         <v>13</v>
       </c>
     </row>
@@ -12340,22 +12340,22 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="b">
+      <c r="B4" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="b">
+      <c r="C4" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -12363,22 +12363,22 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -12386,22 +12386,22 @@
       <c r="A6" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="9" t="s">
         <v>1972</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="9" t="s">
         <v>1972</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -12409,18 +12409,18 @@
       <c r="A7" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8" t="s">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="13" t="s">
         <v>10</v>
       </c>
     </row>
@@ -12446,299 +12446,299 @@
     <row r="15" ht="15.75" customHeight="1"/>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2" t="s">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="14" t="s">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
     </row>
     <row r="24" ht="224.25" customHeight="1">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="H26" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I26" s="14" t="s">
+      <c r="I26" s="6" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I27" s="14" t="s">
+      <c r="I27" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -12929,37 +12929,37 @@
       <c r="A1" s="15" t="s">
         <v>1973</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="4" t="s">
         <v>1974</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="4" t="s">
         <v>1975</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="4" t="s">
         <v>1976</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="4" t="s">
         <v>1977</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="4" t="s">
         <v>1978</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="4" t="s">
         <v>1979</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="4" t="s">
         <v>1980</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="4" t="s">
         <v>1981</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="4" t="s">
         <v>1982</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="4" t="s">
         <v>1983</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="4" t="s">
         <v>1984</v>
       </c>
       <c r="M1" s="21" t="s">
@@ -12968,358 +12968,358 @@
       <c r="N1" s="22" t="s">
         <v>1986</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="4" t="s">
         <v>1987</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="4" t="s">
         <v>1988</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="4" t="s">
         <v>1989</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="4" t="s">
         <v>1990</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="4" t="s">
         <v>1991</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="4" t="s">
         <v>1992</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="4" t="s">
         <v>1993</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="V1" s="4" t="s">
         <v>1994</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="W1" s="4" t="s">
         <v>1995</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="X1" s="4" t="s">
         <v>1996</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Y1" s="4" t="s">
         <v>1997</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="Z1" s="4" t="s">
         <v>1998</v>
       </c>
-      <c r="AA1" s="12" t="s">
+      <c r="AA1" s="4" t="s">
         <v>1999</v>
       </c>
-      <c r="AB1" s="12" t="s">
+      <c r="AB1" s="4" t="s">
         <v>2000</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AC1" s="4" t="s">
         <v>2001</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AD1" s="4" t="s">
         <v>2002</v>
       </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AE1" s="4" t="s">
         <v>2003</v>
       </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AF1" s="4" t="s">
         <v>2004</v>
       </c>
-      <c r="AG1" s="12" t="s">
+      <c r="AG1" s="4" t="s">
         <v>2005</v>
       </c>
-      <c r="AH1" s="12" t="s">
+      <c r="AH1" s="4" t="s">
         <v>2006</v>
       </c>
-      <c r="AI1" s="12" t="s">
+      <c r="AI1" s="4" t="s">
         <v>2007</v>
       </c>
-      <c r="AJ1" s="12" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>2008</v>
       </c>
-      <c r="AK1" s="12" t="s">
+      <c r="AK1" s="4" t="s">
         <v>2009</v>
       </c>
-      <c r="AL1" s="12" t="s">
+      <c r="AL1" s="4" t="s">
         <v>2010</v>
       </c>
-      <c r="AM1" s="12" t="s">
+      <c r="AM1" s="4" t="s">
         <v>2011</v>
       </c>
-      <c r="AN1" s="12" t="s">
+      <c r="AN1" s="4" t="s">
         <v>2012</v>
       </c>
-      <c r="AO1" s="12" t="s">
+      <c r="AO1" s="4" t="s">
         <v>2013</v>
       </c>
-      <c r="AP1" s="12" t="s">
+      <c r="AP1" s="4" t="s">
         <v>2014</v>
       </c>
-      <c r="AQ1" s="12" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>2015</v>
       </c>
-      <c r="AR1" s="12" t="s">
+      <c r="AR1" s="4" t="s">
         <v>2016</v>
       </c>
-      <c r="AS1" s="12" t="s">
+      <c r="AS1" s="4" t="s">
         <v>2017</v>
       </c>
-      <c r="AT1" s="12" t="s">
+      <c r="AT1" s="4" t="s">
         <v>2018</v>
       </c>
-      <c r="AU1" s="12" t="s">
+      <c r="AU1" s="4" t="s">
         <v>2019</v>
       </c>
-      <c r="AV1" s="12" t="s">
+      <c r="AV1" s="4" t="s">
         <v>2020</v>
       </c>
-      <c r="AW1" s="12" t="s">
+      <c r="AW1" s="4" t="s">
         <v>2021</v>
       </c>
-      <c r="AX1" s="12" t="s">
+      <c r="AX1" s="4" t="s">
         <v>2022</v>
       </c>
-      <c r="AY1" s="12" t="s">
+      <c r="AY1" s="4" t="s">
         <v>2023</v>
       </c>
-      <c r="AZ1" s="12" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>2024</v>
       </c>
-      <c r="BA1" s="12" t="s">
+      <c r="BA1" s="4" t="s">
         <v>2025</v>
       </c>
-      <c r="BB1" s="12" t="s">
+      <c r="BB1" s="4" t="s">
         <v>2026</v>
       </c>
-      <c r="BC1" s="12" t="s">
+      <c r="BC1" s="4" t="s">
         <v>2027</v>
       </c>
-      <c r="BD1" s="12" t="s">
+      <c r="BD1" s="4" t="s">
         <v>2028</v>
       </c>
-      <c r="BE1" s="12" t="s">
+      <c r="BE1" s="4" t="s">
         <v>2029</v>
       </c>
-      <c r="BF1" s="12" t="s">
+      <c r="BF1" s="4" t="s">
         <v>2030</v>
       </c>
-      <c r="BG1" s="12" t="s">
+      <c r="BG1" s="4" t="s">
         <v>2031</v>
       </c>
-      <c r="BH1" s="12" t="s">
+      <c r="BH1" s="4" t="s">
         <v>2032</v>
       </c>
-      <c r="BI1" s="12" t="s">
+      <c r="BI1" s="4" t="s">
         <v>2033</v>
       </c>
-      <c r="BJ1" s="12" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>2034</v>
       </c>
-      <c r="BK1" s="12" t="s">
+      <c r="BK1" s="4" t="s">
         <v>2035</v>
       </c>
-      <c r="BL1" s="12" t="s">
+      <c r="BL1" s="4" t="s">
         <v>2036</v>
       </c>
-      <c r="BM1" s="12" t="s">
+      <c r="BM1" s="4" t="s">
         <v>2037</v>
       </c>
-      <c r="BN1" s="12" t="s">
+      <c r="BN1" s="4" t="s">
         <v>2038</v>
       </c>
-      <c r="BO1" s="12" t="s">
+      <c r="BO1" s="4" t="s">
         <v>2039</v>
       </c>
-      <c r="BP1" s="12" t="s">
+      <c r="BP1" s="4" t="s">
         <v>2040</v>
       </c>
-      <c r="BQ1" s="12" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>2041</v>
       </c>
-      <c r="BR1" s="12" t="s">
+      <c r="BR1" s="4" t="s">
         <v>2042</v>
       </c>
-      <c r="BS1" s="12" t="s">
+      <c r="BS1" s="4" t="s">
         <v>2043</v>
       </c>
-      <c r="BT1" s="12" t="s">
+      <c r="BT1" s="4" t="s">
         <v>2044</v>
       </c>
-      <c r="BU1" s="12" t="s">
+      <c r="BU1" s="4" t="s">
         <v>2045</v>
       </c>
-      <c r="BV1" s="12" t="s">
+      <c r="BV1" s="4" t="s">
         <v>2046</v>
       </c>
-      <c r="BW1" s="12" t="s">
+      <c r="BW1" s="4" t="s">
         <v>2047</v>
       </c>
-      <c r="BX1" s="12" t="s">
+      <c r="BX1" s="4" t="s">
         <v>2048</v>
       </c>
-      <c r="BY1" s="12" t="s">
+      <c r="BY1" s="4" t="s">
         <v>2049</v>
       </c>
-      <c r="BZ1" s="12" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>2050</v>
       </c>
-      <c r="CA1" s="12" t="s">
+      <c r="CA1" s="4" t="s">
         <v>2051</v>
       </c>
-      <c r="CB1" s="12" t="s">
+      <c r="CB1" s="4" t="s">
         <v>2052</v>
       </c>
-      <c r="CC1" s="12" t="s">
+      <c r="CC1" s="4" t="s">
         <v>2053</v>
       </c>
-      <c r="CD1" s="12" t="s">
+      <c r="CD1" s="4" t="s">
         <v>2054</v>
       </c>
-      <c r="CE1" s="12" t="s">
+      <c r="CE1" s="4" t="s">
         <v>2055</v>
       </c>
-      <c r="CF1" s="12" t="s">
+      <c r="CF1" s="4" t="s">
         <v>2056</v>
       </c>
-      <c r="CG1" s="12" t="s">
+      <c r="CG1" s="4" t="s">
         <v>2057</v>
       </c>
-      <c r="CH1" s="12" t="s">
+      <c r="CH1" s="4" t="s">
         <v>2058</v>
       </c>
-      <c r="CI1" s="12" t="s">
+      <c r="CI1" s="4" t="s">
         <v>2059</v>
       </c>
-      <c r="CJ1" s="12" t="s">
+      <c r="CJ1" s="4" t="s">
         <v>2060</v>
       </c>
-      <c r="CK1" s="12" t="s">
+      <c r="CK1" s="4" t="s">
         <v>2061</v>
       </c>
-      <c r="CL1" s="12" t="s">
+      <c r="CL1" s="4" t="s">
         <v>2062</v>
       </c>
-      <c r="CM1" s="12" t="s">
+      <c r="CM1" s="4" t="s">
         <v>2063</v>
       </c>
-      <c r="CN1" s="12" t="s">
+      <c r="CN1" s="4" t="s">
         <v>2064</v>
       </c>
-      <c r="CO1" s="12" t="s">
+      <c r="CO1" s="4" t="s">
         <v>2065</v>
       </c>
-      <c r="CP1" s="12" t="s">
+      <c r="CP1" s="4" t="s">
         <v>2066</v>
       </c>
-      <c r="CQ1" s="12" t="s">
+      <c r="CQ1" s="4" t="s">
         <v>2067</v>
       </c>
-      <c r="CR1" s="12" t="s">
+      <c r="CR1" s="4" t="s">
         <v>2068</v>
       </c>
-      <c r="CS1" s="12" t="s">
+      <c r="CS1" s="4" t="s">
         <v>2069</v>
       </c>
-      <c r="CT1" s="12" t="s">
+      <c r="CT1" s="4" t="s">
         <v>2070</v>
       </c>
-      <c r="CU1" s="12" t="s">
+      <c r="CU1" s="4" t="s">
         <v>2071</v>
       </c>
-      <c r="CV1" s="12" t="s">
+      <c r="CV1" s="4" t="s">
         <v>2072</v>
       </c>
-      <c r="CW1" s="12" t="s">
+      <c r="CW1" s="4" t="s">
         <v>2073</v>
       </c>
-      <c r="CX1" s="12" t="s">
+      <c r="CX1" s="4" t="s">
         <v>2074</v>
       </c>
-      <c r="CY1" s="12" t="s">
+      <c r="CY1" s="4" t="s">
         <v>2075</v>
       </c>
-      <c r="CZ1" s="12" t="s">
+      <c r="CZ1" s="4" t="s">
         <v>2076</v>
       </c>
-      <c r="DA1" s="12" t="s">
+      <c r="DA1" s="4" t="s">
         <v>2077</v>
       </c>
-      <c r="DB1" s="12" t="s">
+      <c r="DB1" s="4" t="s">
         <v>2078</v>
       </c>
-      <c r="DC1" s="12" t="s">
+      <c r="DC1" s="4" t="s">
         <v>2079</v>
       </c>
-      <c r="DD1" s="12" t="s">
+      <c r="DD1" s="4" t="s">
         <v>2080</v>
       </c>
-      <c r="DE1" s="12" t="s">
+      <c r="DE1" s="4" t="s">
         <v>2081</v>
       </c>
       <c r="DF1" s="15" t="s">
         <v>2082</v>
       </c>
-      <c r="DG1" s="12" t="s">
+      <c r="DG1" s="4" t="s">
         <v>2083</v>
       </c>
-      <c r="DH1" s="12" t="s">
+      <c r="DH1" s="4" t="s">
         <v>2084</v>
       </c>
-      <c r="DI1" s="12" t="s">
+      <c r="DI1" s="4" t="s">
         <v>2085</v>
       </c>
-      <c r="DJ1" s="12" t="s">
+      <c r="DJ1" s="4" t="s">
         <v>2086</v>
       </c>
-      <c r="DK1" s="12" t="s">
+      <c r="DK1" s="4" t="s">
         <v>2087</v>
       </c>
-      <c r="DL1" s="12" t="s">
+      <c r="DL1" s="4" t="s">
         <v>2088</v>
       </c>
-      <c r="DM1" s="12" t="s">
+      <c r="DM1" s="4" t="s">
         <v>2089</v>
       </c>
-      <c r="DN1" s="12" t="s">
+      <c r="DN1" s="4" t="s">
         <v>2090</v>
       </c>
-      <c r="DO1" s="12" t="s">
+      <c r="DO1" s="4" t="s">
         <v>2091</v>
       </c>
-      <c r="DP1" s="12" t="s">
+      <c r="DP1" s="4" t="s">
         <v>2092</v>
       </c>
-      <c r="DQ1" s="12" t="s">
+      <c r="DQ1" s="4" t="s">
         <v>2093</v>
       </c>
-      <c r="DR1" s="12" t="s">
+      <c r="DR1" s="4" t="s">
         <v>2094</v>
       </c>
-      <c r="DS1" s="12" t="s">
+      <c r="DS1" s="4" t="s">
         <v>2095</v>
       </c>
-      <c r="DT1" s="12" t="s">
+      <c r="DT1" s="4" t="s">
         <v>2096</v>
       </c>
-      <c r="DU1" s="12" t="s">
+      <c r="DU1" s="4" t="s">
         <v>2097</v>
       </c>
-      <c r="DV1" s="12" t="s">
+      <c r="DV1" s="4" t="s">
         <v>2098</v>
       </c>
-      <c r="DW1" s="12" t="s">
+      <c r="DW1" s="4" t="s">
         <v>2099</v>
       </c>
-      <c r="DX1" s="12" t="s">
+      <c r="DX1" s="4" t="s">
         <v>2100</v>
       </c>
-      <c r="DY1" s="12" t="s">
+      <c r="DY1" s="4" t="s">
         <v>2101</v>
       </c>
-      <c r="DZ1" s="12" t="s">
+      <c r="DZ1" s="4" t="s">
         <v>2102</v>
       </c>
-      <c r="EA1" s="12" t="s">
+      <c r="EA1" s="4" t="s">
         <v>2103</v>
       </c>
-      <c r="EB1" s="12" t="s">
+      <c r="EB1" s="4" t="s">
         <v>2104</v>
       </c>
       <c r="EC1" t="s">

</xml_diff>